<commit_message>
GIT TESTING FROM LOCAL Signed-off-by: Rajesh kumar <rkhinditron@gmail.com>
</commit_message>
<xml_diff>
--- a/PrepMaster.xlsx
+++ b/PrepMaster.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="690" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="690"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -4054,7 +4054,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="221">
   <si>
     <t>File Name</t>
   </si>
@@ -4853,6 +4853,9 @@
   </si>
   <si>
     <t xml:space="preserve">1 = BOOL </t>
+  </si>
+  <si>
+    <t>TEST GIT GUI SOFTWARE</t>
   </si>
 </sst>
 </file>
@@ -4948,7 +4951,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4970,6 +4973,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5234,7 +5243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5309,6 +5318,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5348,11 +5363,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6364,10 +6376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B51"/>
+  <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6610,17 +6622,62 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>176</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="43"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="43"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="43"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A54:F58"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6903,7 +6960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -6917,17 +6974,17 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="11" t="s">
         <v>95</v>
       </c>
@@ -6951,7 +7008,7 @@
       <c r="E5" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="29" t="s">
         <v>219</v>
       </c>
     </row>
@@ -6968,7 +7025,7 @@
       <c r="E6" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="28" t="s">
         <v>213</v>
       </c>
     </row>
@@ -6985,7 +7042,7 @@
       <c r="E7" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="28" t="s">
         <v>214</v>
       </c>
     </row>
@@ -7002,7 +7059,7 @@
       <c r="E8" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="28" t="s">
         <v>215</v>
       </c>
     </row>
@@ -7019,7 +7076,7 @@
       <c r="E9" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="28" t="s">
         <v>216</v>
       </c>
     </row>
@@ -7036,7 +7093,7 @@
       <c r="E10" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="28" t="s">
         <v>217</v>
       </c>
     </row>
@@ -7053,7 +7110,7 @@
       <c r="E11" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="28" t="s">
         <v>218</v>
       </c>
     </row>
@@ -7231,45 +7288,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="36"/>
+      <c r="AM2" s="37"/>
     </row>
     <row r="3" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C3" s="25" t="s">
@@ -7278,51 +7335,51 @@
       <c r="D3" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="36" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="36" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="36" t="s">
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="36" t="s">
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
-      <c r="AM3" s="38"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="40"/>
     </row>
     <row r="4" spans="2:39" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
@@ -8362,45 +8419,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="41"/>
+      <c r="AH2" s="41"/>
+      <c r="AI2" s="41"/>
+      <c r="AJ2" s="41"/>
+      <c r="AK2" s="41"/>
+      <c r="AL2" s="41"/>
+      <c r="AM2" s="41"/>
     </row>
     <row r="3" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C3" s="25" t="s">
@@ -8409,51 +8466,51 @@
       <c r="D3" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="36" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="36" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="36" t="s">
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="40" t="s">
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="40"/>
-      <c r="AF3" s="40"/>
-      <c r="AG3" s="40"/>
-      <c r="AH3" s="40"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="40"/>
-      <c r="AK3" s="40"/>
-      <c r="AL3" s="40"/>
-      <c r="AM3" s="40"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="42"/>
+      <c r="AF3" s="42"/>
+      <c r="AG3" s="42"/>
+      <c r="AH3" s="42"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AM3" s="42"/>
     </row>
     <row r="4" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">

</xml_diff>